<commit_message>
GPLIM-2588 Fix spreadsheet headers.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/manifest-upload/duplicates/good-manifest-1.xlsx
+++ b/mercury/src/test/resources/testdata/manifest-upload/duplicates/good-manifest-1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="280" windowWidth="25600" windowHeight="20460"/>
@@ -246,12 +246,6 @@
     <t>24-Apr-2012</t>
   </si>
   <si>
-    <t>T/N</t>
-  </si>
-  <si>
-    <t>Sample ID</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -262,6 +256,12 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>Specimen_Number</t>
+  </si>
+  <si>
+    <t>SAMPLE_TYPE</t>
   </si>
 </sst>
 </file>
@@ -730,7 +730,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -744,7 +744,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -770,7 +770,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -779,7 +779,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -790,7 +790,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -799,7 +799,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -810,7 +810,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -819,7 +819,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -830,7 +830,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -839,7 +839,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -850,7 +850,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
@@ -859,7 +859,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -870,7 +870,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>22</v>
@@ -879,7 +879,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -890,7 +890,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>25</v>
@@ -899,7 +899,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -910,7 +910,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>28</v>
@@ -919,7 +919,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -930,7 +930,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>31</v>
@@ -939,7 +939,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -950,7 +950,7 @@
         <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>34</v>
@@ -959,7 +959,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -970,7 +970,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>37</v>
@@ -979,7 +979,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -990,7 +990,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>40</v>
@@ -999,7 +999,7 @@
         <v>7</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1010,7 +1010,7 @@
         <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>43</v>
@@ -1019,7 +1019,7 @@
         <v>7</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1030,7 +1030,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>46</v>
@@ -1039,7 +1039,7 @@
         <v>7</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1050,7 +1050,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>49</v>
@@ -1059,7 +1059,7 @@
         <v>7</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1070,7 +1070,7 @@
         <v>51</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>52</v>
@@ -1079,7 +1079,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1090,7 +1090,7 @@
         <v>54</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>55</v>
@@ -1099,7 +1099,7 @@
         <v>7</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1110,7 +1110,7 @@
         <v>57</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>58</v>
@@ -1119,7 +1119,7 @@
         <v>7</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1130,7 +1130,7 @@
         <v>60</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>61</v>
@@ -1139,7 +1139,7 @@
         <v>7</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1150,7 +1150,7 @@
         <v>63</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>64</v>
@@ -1159,7 +1159,7 @@
         <v>7</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1170,7 +1170,7 @@
         <v>66</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>67</v>
@@ -1179,7 +1179,7 @@
         <v>7</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1190,7 +1190,7 @@
         <v>69</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>70</v>
@@ -1199,7 +1199,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1210,7 +1210,7 @@
         <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>73</v>
@@ -1219,7 +1219,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>